<commit_message>
final changes before presentation
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kouluhommat\OneDrive - Oulun ammattikorkeakoulu\DevBasicSkills2019-16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venla\Documents\DevBasicSkills2019-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F9D81C-CE98-4F15-A873-E67D22A2D6CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18135" windowHeight="10725"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>DATE:</t>
   </si>
@@ -63,12 +70,45 @@
   </si>
   <si>
     <t>Joni:</t>
+  </si>
+  <si>
+    <t>Setting development enviorment</t>
+  </si>
+  <si>
+    <t>Creating initial sass folder and files</t>
+  </si>
+  <si>
+    <t>Creating header</t>
+  </si>
+  <si>
+    <t>Created 6 cards where to select functions</t>
+  </si>
+  <si>
+    <t>Styled 6 cards with headings and svg icons</t>
+  </si>
+  <si>
+    <t>Created popup window component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added popup to all six buttons  </t>
+  </si>
+  <si>
+    <t>Styled functions inside popup</t>
+  </si>
+  <si>
+    <t>#########</t>
+  </si>
+  <si>
+    <t>########</t>
+  </si>
+  <si>
+    <t>Footer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +158,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,26 +435,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -422,7 +462,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -442,11 +482,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>43802</v>
       </c>
@@ -459,9 +499,14 @@
       <c r="G5" s="1">
         <v>43802</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>43803</v>
       </c>
@@ -474,9 +519,14 @@
       <c r="G6" s="1">
         <v>43803</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>43804</v>
       </c>
@@ -489,9 +539,14 @@
       <c r="G7" s="1">
         <v>43804</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>43805</v>
       </c>
@@ -501,7 +556,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>43806</v>
       </c>
@@ -516,7 +571,7 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>43807</v>
       </c>
@@ -524,9 +579,14 @@
       <c r="G10" s="1">
         <v>43807</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="2">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>43808</v>
       </c>
@@ -539,9 +599,14 @@
       <c r="G11" s="1">
         <v>43808</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>43809</v>
       </c>
@@ -551,7 +616,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>43810</v>
       </c>
@@ -564,9 +629,14 @@
       <c r="G13" s="1">
         <v>43810</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>43811</v>
       </c>
@@ -579,9 +649,14 @@
       <c r="G14" s="1">
         <v>43811</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>43812</v>
       </c>
@@ -591,7 +666,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>43813</v>
       </c>
@@ -599,9 +674,14 @@
       <c r="G16" s="1">
         <v>43813</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <v>43814</v>
       </c>
@@ -614,9 +694,14 @@
       <c r="G17" s="1">
         <v>43814</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>43815</v>
       </c>
@@ -629,9 +714,14 @@
       <c r="G18" s="1">
         <v>43815</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>43816</v>
       </c>
@@ -639,21 +729,42 @@
       <c r="G19" s="1">
         <v>43816</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="2">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -667,29 +778,29 @@
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="4">
-        <f>SUM(H5:H20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <f>SUM(H5:H21)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C30" s="2"/>
     </row>
   </sheetData>

</xml_diff>